<commit_message>
added reference for AXDW* users
</commit_message>
<xml_diff>
--- a/LBD Deployment Helper - 4 Node.xlsx
+++ b/LBD Deployment Helper - 4 Node.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan.Clouse\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan.Clouse\Downloads\LBDDeploymentHelper-master\LBDDeploymentHelper-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFF0152-D8D1-40A0-BDEE-6354ED73ECA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69278ABB-96D6-4DBB-B9B9-3E55FA621C5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>DNS Name</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Not a Microsoft supported deployment topology</t>
+  </si>
+  <si>
+    <t>AXDWAdmin</t>
+  </si>
+  <si>
+    <t>AXDWRuntimeuser</t>
   </si>
 </sst>
 </file>
@@ -316,11 +322,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -358,8 +365,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46314192-5314-4C6A-B86F-54005C53D21C}" name="Table33" displayName="Table33" ref="A12:D19" totalsRowShown="0">
-  <autoFilter ref="A12:D19" xr:uid="{FF38BC0C-144F-4D95-9AA6-C5574C1DD416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46314192-5314-4C6A-B86F-54005C53D21C}" name="Table33" displayName="Table33" ref="A12:D21" totalsRowShown="0">
+  <autoFilter ref="A12:D21" xr:uid="{FF38BC0C-144F-4D95-9AA6-C5574C1DD416}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B2AB29A1-F5CD-4846-BB24-ED42F46BEA4D}" name="Name"/>
     <tableColumn id="2" xr3:uid="{70E48012-DA42-4A1B-8D86-A6EBD6A59220}" name="Account Name" dataDxfId="0">
@@ -679,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A87E3A0-AE97-4BFF-831F-BBF3B46CBBC6}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1038,38 @@
       </c>
       <c r="D19" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f>LEFT(A20,4) &amp; $G$2 &amp; MID(A20,5,10)</f>
+        <v>AXDWTESTAdmin</v>
+      </c>
+      <c r="C20" t="str">
+        <f xml:space="preserve"> LEFT(A20,4) &amp; $G$2 &amp; MID(A20,5,10)</f>
+        <v>AXDWTESTAdmin</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f>LEFT(A21,4) &amp; $G$2 &amp; MID(A21,5,11)</f>
+        <v>AXDWTESTRuntimeuser</v>
+      </c>
+      <c r="C21" t="str">
+        <f xml:space="preserve"> LEFT(A21,4) &amp; $G$2 &amp; MID(A21,5,11)</f>
+        <v>AXDWTESTRuntimeuser</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>